<commit_message>
Save output of the model and hidden layer output must be repared
</commit_message>
<xml_diff>
--- a/Tesis/Resultados/Escalon/AC/ACOSTADO_Derecho_layer_0.xlsx
+++ b/Tesis/Resultados/Escalon/AC/ACOSTADO_Derecho_layer_0.xlsx
@@ -31,100 +31,100 @@
     <t>W_o</t>
   </si>
   <si>
-    <t>[-0.4308982789516449]</t>
-  </si>
-  <si>
-    <t>[0.37297728657722473]</t>
-  </si>
-  <si>
-    <t>[-0.3001527488231659]</t>
-  </si>
-  <si>
-    <t>[0.353486567735672]</t>
-  </si>
-  <si>
-    <t>[0.42509666085243225]</t>
-  </si>
-  <si>
-    <t>[0.4294171631336212]</t>
-  </si>
-  <si>
-    <t>[-0.34978753328323364]</t>
-  </si>
-  <si>
-    <t>[-0.20894187688827515]</t>
-  </si>
-  <si>
-    <t>[-0.19233103096485138]</t>
-  </si>
-  <si>
-    <t>[0.2761528491973877]</t>
-  </si>
-  <si>
-    <t>[-0.42732319235801697]</t>
-  </si>
-  <si>
-    <t>[0.12843012809753418]</t>
-  </si>
-  <si>
-    <t>[0.4015253782272339]</t>
-  </si>
-  <si>
-    <t>[0.0817883238196373]</t>
-  </si>
-  <si>
-    <t>[-0.14602111279964447]</t>
-  </si>
-  <si>
-    <t>[0.15317866206169128]</t>
-  </si>
-  <si>
-    <t>[-0.3582090437412262]</t>
-  </si>
-  <si>
-    <t>[-0.21189525723457336]</t>
-  </si>
-  <si>
-    <t>[-0.5767087340354919]</t>
-  </si>
-  <si>
-    <t>[0.2620094120502472]</t>
-  </si>
-  <si>
-    <t>[0.5661368370056152]</t>
-  </si>
-  <si>
-    <t>[0.3973403871059418]</t>
-  </si>
-  <si>
-    <t>[-0.5574327707290649]</t>
-  </si>
-  <si>
-    <t>[-0.3618442714214325]</t>
-  </si>
-  <si>
-    <t>[0.12723568081855774]</t>
-  </si>
-  <si>
-    <t>[-0.29695358872413635]</t>
-  </si>
-  <si>
-    <t>[0.2233867198228836]</t>
-  </si>
-  <si>
-    <t>[-0.5522747039794922]</t>
-  </si>
-  <si>
-    <t>[-0.41363438963890076]</t>
-  </si>
-  <si>
-    <t>[0.21489247679710388]</t>
-  </si>
-  <si>
-    <t>[0.4706386923789978]</t>
-  </si>
-  <si>
-    <t>[0.4193612039089203]</t>
+    <t>[-0.43088582158088684]</t>
+  </si>
+  <si>
+    <t>[0.3729703724384308]</t>
+  </si>
+  <si>
+    <t>[-0.3001411557197571]</t>
+  </si>
+  <si>
+    <t>[0.35348230600357056]</t>
+  </si>
+  <si>
+    <t>[0.425092875957489]</t>
+  </si>
+  <si>
+    <t>[0.42943623661994934]</t>
+  </si>
+  <si>
+    <t>[-0.34978681802749634]</t>
+  </si>
+  <si>
+    <t>[-0.20894892513751984]</t>
+  </si>
+  <si>
+    <t>[-0.19233684241771698]</t>
+  </si>
+  <si>
+    <t>[0.27616775035858154]</t>
+  </si>
+  <si>
+    <t>[-0.4273335635662079]</t>
+  </si>
+  <si>
+    <t>[0.1284339427947998]</t>
+  </si>
+  <si>
+    <t>[0.40152812004089355]</t>
+  </si>
+  <si>
+    <t>[0.08179422467947006]</t>
+  </si>
+  <si>
+    <t>[-0.14603085815906525]</t>
+  </si>
+  <si>
+    <t>[0.15319420397281647]</t>
+  </si>
+  <si>
+    <t>[-0.3582150638103485]</t>
+  </si>
+  <si>
+    <t>[-0.2118871957063675]</t>
+  </si>
+  <si>
+    <t>[-0.5767174363136292]</t>
+  </si>
+  <si>
+    <t>[0.2620072662830353]</t>
+  </si>
+  <si>
+    <t>[0.5661380290985107]</t>
+  </si>
+  <si>
+    <t>[0.39734867215156555]</t>
+  </si>
+  <si>
+    <t>[-0.5574347972869873]</t>
+  </si>
+  <si>
+    <t>[-0.3618444800376892]</t>
+  </si>
+  <si>
+    <t>[0.12722600996494293]</t>
+  </si>
+  <si>
+    <t>[-0.2969455420970917]</t>
+  </si>
+  <si>
+    <t>[0.22338248789310455]</t>
+  </si>
+  <si>
+    <t>[-0.5522904396057129]</t>
+  </si>
+  <si>
+    <t>[-0.4136379063129425]</t>
+  </si>
+  <si>
+    <t>[0.2149055004119873]</t>
+  </si>
+  <si>
+    <t>[0.47065725922584534]</t>
+  </si>
+  <si>
+    <t>[0.4193534851074219]</t>
   </si>
   <si>
     <t>U_i</t>
@@ -139,772 +139,772 @@
     <t>U_o</t>
   </si>
   <si>
-    <t>[-0.34543463587760925]</t>
-  </si>
-  <si>
-    <t>[0.2500840723514557]</t>
-  </si>
-  <si>
-    <t>[-0.34761109948158264]</t>
-  </si>
-  <si>
-    <t>[0.06382187455892563]</t>
-  </si>
-  <si>
-    <t>[0.13814932107925415]</t>
-  </si>
-  <si>
-    <t>[0.18671131134033203]</t>
-  </si>
-  <si>
-    <t>[-0.21300312876701355]</t>
-  </si>
-  <si>
-    <t>[-0.12272234261035919]</t>
-  </si>
-  <si>
-    <t>[-0.09077155590057373]</t>
-  </si>
-  <si>
-    <t>[0.32528042793273926]</t>
-  </si>
-  <si>
-    <t>[-0.07045265287160873]</t>
-  </si>
-  <si>
-    <t>[-0.013281533494591713]</t>
-  </si>
-  <si>
-    <t>[0.3339404761791229]</t>
-  </si>
-  <si>
-    <t>[0.019299354404211044]</t>
-  </si>
-  <si>
-    <t>[0.05807160213589668]</t>
-  </si>
-  <si>
-    <t>[-0.29449695348739624]</t>
-  </si>
-  <si>
-    <t>[-0.11435650289058685]</t>
-  </si>
-  <si>
-    <t>[0.2748285233974457]</t>
-  </si>
-  <si>
-    <t>[0.1537516862154007]</t>
-  </si>
-  <si>
-    <t>[0.15438047051429749]</t>
-  </si>
-  <si>
-    <t>[-0.01602817326784134]</t>
-  </si>
-  <si>
-    <t>[-0.18051333725452423]</t>
-  </si>
-  <si>
-    <t>[-0.12695752084255219]</t>
-  </si>
-  <si>
-    <t>[-0.09566106647253036]</t>
-  </si>
-  <si>
-    <t>[-0.19331814348697662]</t>
-  </si>
-  <si>
-    <t>[0.3410658538341522]</t>
-  </si>
-  <si>
-    <t>[0.6332622170448303]</t>
-  </si>
-  <si>
-    <t>[-0.13934646546840668]</t>
-  </si>
-  <si>
-    <t>[0.05358244478702545]</t>
-  </si>
-  <si>
-    <t>[0.049584921449422836]</t>
-  </si>
-  <si>
-    <t>[0.00649452768266201]</t>
-  </si>
-  <si>
-    <t>[0.10014266520738602]</t>
-  </si>
-  <si>
-    <t>[-0.23448318243026733]</t>
-  </si>
-  <si>
-    <t>[0.026521282270550728]</t>
-  </si>
-  <si>
-    <t>[-0.19026437401771545]</t>
-  </si>
-  <si>
-    <t>[0.16239547729492188]</t>
-  </si>
-  <si>
-    <t>[0.23259998857975006]</t>
-  </si>
-  <si>
-    <t>[-0.1996530443429947]</t>
-  </si>
-  <si>
-    <t>[0.038768310099840164]</t>
-  </si>
-  <si>
-    <t>[-0.42266860604286194]</t>
-  </si>
-  <si>
-    <t>[-0.3251263499259949]</t>
-  </si>
-  <si>
-    <t>[-0.1282753050327301]</t>
-  </si>
-  <si>
-    <t>[-0.03650406002998352]</t>
-  </si>
-  <si>
-    <t>[0.23653747141361237]</t>
-  </si>
-  <si>
-    <t>[0.0016216719523072243]</t>
-  </si>
-  <si>
-    <t>[0.05912836641073227]</t>
-  </si>
-  <si>
-    <t>[0.14655719697475433]</t>
-  </si>
-  <si>
-    <t>[-0.2684416174888611]</t>
-  </si>
-  <si>
-    <t>[0.038994308561086655]</t>
-  </si>
-  <si>
-    <t>[0.01724928431212902]</t>
-  </si>
-  <si>
-    <t>[0.05462685599923134]</t>
-  </si>
-  <si>
-    <t>[0.45923206210136414]</t>
-  </si>
-  <si>
-    <t>[-0.19057564437389374]</t>
-  </si>
-  <si>
-    <t>[0.03780803456902504]</t>
-  </si>
-  <si>
-    <t>[0.02976115792989731]</t>
-  </si>
-  <si>
-    <t>[-0.09160053730010986]</t>
-  </si>
-  <si>
-    <t>[0.07949556410312653]</t>
-  </si>
-  <si>
-    <t>[0.16051191091537476]</t>
-  </si>
-  <si>
-    <t>[0.03207765147089958]</t>
-  </si>
-  <si>
-    <t>[-0.1825844645500183]</t>
-  </si>
-  <si>
-    <t>[-0.504002571105957]</t>
-  </si>
-  <si>
-    <t>[0.12201295047998428]</t>
-  </si>
-  <si>
-    <t>[-0.2822120487689972]</t>
-  </si>
-  <si>
-    <t>[0.1816176176071167]</t>
-  </si>
-  <si>
-    <t>[-0.11548560857772827]</t>
-  </si>
-  <si>
-    <t>[0.05141819640994072]</t>
-  </si>
-  <si>
-    <t>[-0.4878460168838501]</t>
-  </si>
-  <si>
-    <t>[0.2951414883136749]</t>
-  </si>
-  <si>
-    <t>[-0.18872687220573425]</t>
-  </si>
-  <si>
-    <t>[0.15525290369987488]</t>
-  </si>
-  <si>
-    <t>[0.005476953461766243]</t>
-  </si>
-  <si>
-    <t>[0.1883886307477951]</t>
-  </si>
-  <si>
-    <t>[0.05883084982633591]</t>
-  </si>
-  <si>
-    <t>[-0.12392690032720566]</t>
-  </si>
-  <si>
-    <t>[-0.10861095041036606]</t>
-  </si>
-  <si>
-    <t>[0.10734936594963074]</t>
-  </si>
-  <si>
-    <t>[0.26173341274261475]</t>
-  </si>
-  <si>
-    <t>[0.1981719583272934]</t>
-  </si>
-  <si>
-    <t>[-0.23301967978477478]</t>
-  </si>
-  <si>
-    <t>[0.12271483242511749]</t>
-  </si>
-  <si>
-    <t>[-0.2552506923675537]</t>
-  </si>
-  <si>
-    <t>[0.34721750020980835]</t>
-  </si>
-  <si>
-    <t>[-0.3652108609676361]</t>
-  </si>
-  <si>
-    <t>[0.3008870780467987]</t>
-  </si>
-  <si>
-    <t>[-0.020524103194475174]</t>
-  </si>
-  <si>
-    <t>[0.07886848598718643]</t>
-  </si>
-  <si>
-    <t>[-0.14770165085792542]</t>
-  </si>
-  <si>
-    <t>[-0.2089526653289795]</t>
-  </si>
-  <si>
-    <t>[0.36796292662620544]</t>
-  </si>
-  <si>
-    <t>[-0.013033337891101837]</t>
-  </si>
-  <si>
-    <t>[0.25408098101615906]</t>
-  </si>
-  <si>
-    <t>[-0.25585952401161194]</t>
-  </si>
-  <si>
-    <t>[-0.23858307301998138]</t>
-  </si>
-  <si>
-    <t>[-0.08630608022212982]</t>
-  </si>
-  <si>
-    <t>[-0.00910449679940939]</t>
-  </si>
-  <si>
-    <t>[0.01571277156472206]</t>
-  </si>
-  <si>
-    <t>[0.19204333424568176]</t>
-  </si>
-  <si>
-    <t>[-0.5275287628173828]</t>
-  </si>
-  <si>
-    <t>[-0.3380148708820343]</t>
-  </si>
-  <si>
-    <t>[-0.1043819934129715]</t>
-  </si>
-  <si>
-    <t>[-0.08539528399705887]</t>
-  </si>
-  <si>
-    <t>[0.01715599186718464]</t>
-  </si>
-  <si>
-    <t>[0.19110295176506042]</t>
-  </si>
-  <si>
-    <t>[0.23033662140369415]</t>
-  </si>
-  <si>
-    <t>[-0.1523798257112503]</t>
-  </si>
-  <si>
-    <t>[0.10867182910442352]</t>
-  </si>
-  <si>
-    <t>[0.027277320623397827]</t>
-  </si>
-  <si>
-    <t>[-0.2603587508201599]</t>
-  </si>
-  <si>
-    <t>[-0.014453420415520668]</t>
-  </si>
-  <si>
-    <t>[0.11087260395288467]</t>
-  </si>
-  <si>
-    <t>[-0.16211651265621185]</t>
-  </si>
-  <si>
-    <t>[-0.0938449278473854]</t>
-  </si>
-  <si>
-    <t>[0.04380853474140167]</t>
-  </si>
-  <si>
-    <t>[-0.11570728570222855]</t>
-  </si>
-  <si>
-    <t>[-0.009848322719335556]</t>
-  </si>
-  <si>
-    <t>[-0.33402976393699646]</t>
-  </si>
-  <si>
-    <t>[-0.15595895051956177]</t>
-  </si>
-  <si>
-    <t>[-0.1430124193429947]</t>
-  </si>
-  <si>
-    <t>[0.21257396042346954]</t>
-  </si>
-  <si>
-    <t>[0.2831897735595703]</t>
-  </si>
-  <si>
-    <t>[-0.2624204158782959]</t>
-  </si>
-  <si>
-    <t>[-0.020112305879592896]</t>
-  </si>
-  <si>
-    <t>[-0.25059860944747925]</t>
-  </si>
-  <si>
-    <t>[0.16298359632492065]</t>
-  </si>
-  <si>
-    <t>[0.1881539672613144]</t>
-  </si>
-  <si>
-    <t>[0.25194403529167175]</t>
-  </si>
-  <si>
-    <t>[-0.03590879216790199]</t>
-  </si>
-  <si>
-    <t>[-0.25965869426727295]</t>
-  </si>
-  <si>
-    <t>[-0.28732192516326904]</t>
-  </si>
-  <si>
-    <t>[0.10152877122163773]</t>
-  </si>
-  <si>
-    <t>[-0.08600347489118576]</t>
-  </si>
-  <si>
-    <t>[0.1493173986673355]</t>
-  </si>
-  <si>
-    <t>[0.14844243228435516]</t>
-  </si>
-  <si>
-    <t>[0.04284374788403511]</t>
-  </si>
-  <si>
-    <t>[0.16556183993816376]</t>
-  </si>
-  <si>
-    <t>[0.2499874383211136]</t>
-  </si>
-  <si>
-    <t>[0.10421169549226761]</t>
-  </si>
-  <si>
-    <t>[-0.08068497478961945]</t>
-  </si>
-  <si>
-    <t>[0.4349835216999054]</t>
-  </si>
-  <si>
-    <t>[0.04501109570264816]</t>
-  </si>
-  <si>
-    <t>[0.15009647607803345]</t>
-  </si>
-  <si>
-    <t>[0.11466006934642792]</t>
-  </si>
-  <si>
-    <t>[-0.04331843927502632]</t>
-  </si>
-  <si>
-    <t>[-0.07018258422613144]</t>
-  </si>
-  <si>
-    <t>[0.47388818860054016]</t>
-  </si>
-  <si>
-    <t>[0.2715158462524414]</t>
-  </si>
-  <si>
-    <t>[0.09529048204421997]</t>
-  </si>
-  <si>
-    <t>[0.19463498890399933]</t>
-  </si>
-  <si>
-    <t>[0.045526452362537384]</t>
-  </si>
-  <si>
-    <t>[-0.24672070145606995]</t>
-  </si>
-  <si>
-    <t>[-0.16258926689624786]</t>
-  </si>
-  <si>
-    <t>[-0.07246150821447372]</t>
-  </si>
-  <si>
-    <t>[0.11494912952184677]</t>
-  </si>
-  <si>
-    <t>[0.016923364251852036]</t>
-  </si>
-  <si>
-    <t>[0.04942508041858673]</t>
-  </si>
-  <si>
-    <t>[-0.14521192014217377]</t>
-  </si>
-  <si>
-    <t>[-0.02854103595018387]</t>
-  </si>
-  <si>
-    <t>[-0.1109384149312973]</t>
-  </si>
-  <si>
-    <t>[-0.11026379466056824]</t>
-  </si>
-  <si>
-    <t>[0.23800697922706604]</t>
-  </si>
-  <si>
-    <t>[-0.40473657846450806]</t>
-  </si>
-  <si>
-    <t>[0.1998320072889328]</t>
-  </si>
-  <si>
-    <t>[-0.340902179479599]</t>
-  </si>
-  <si>
-    <t>[0.41212087869644165]</t>
-  </si>
-  <si>
-    <t>[-0.11143391579389572]</t>
-  </si>
-  <si>
-    <t>[-0.08208579570055008]</t>
-  </si>
-  <si>
-    <t>[0.1373095065355301]</t>
-  </si>
-  <si>
-    <t>[-0.10270445793867111]</t>
-  </si>
-  <si>
-    <t>[-0.022793933749198914]</t>
-  </si>
-  <si>
-    <t>[0.018579227849841118]</t>
-  </si>
-  <si>
-    <t>[-0.10515978187322617]</t>
-  </si>
-  <si>
-    <t>[-0.0009548840462230146]</t>
-  </si>
-  <si>
-    <t>[0.3555910587310791]</t>
-  </si>
-  <si>
-    <t>[-0.3193177580833435]</t>
-  </si>
-  <si>
-    <t>[0.06175171211361885]</t>
-  </si>
-  <si>
-    <t>[0.25633591413497925]</t>
-  </si>
-  <si>
-    <t>[-0.03228103369474411]</t>
-  </si>
-  <si>
-    <t>[-0.20581354200839996]</t>
-  </si>
-  <si>
-    <t>[-0.15528178215026855]</t>
-  </si>
-  <si>
-    <t>[-0.03965394198894501]</t>
-  </si>
-  <si>
-    <t>[0.08639127761125565]</t>
-  </si>
-  <si>
-    <t>[-0.16189467906951904]</t>
-  </si>
-  <si>
-    <t>[-0.06071566045284271]</t>
-  </si>
-  <si>
-    <t>[-0.30268481373786926]</t>
-  </si>
-  <si>
-    <t>[-0.11742395162582397]</t>
-  </si>
-  <si>
-    <t>[0.2994190454483032]</t>
-  </si>
-  <si>
-    <t>[0.0002037680387729779]</t>
-  </si>
-  <si>
-    <t>[-0.556277334690094]</t>
-  </si>
-  <si>
-    <t>[-0.15076883137226105]</t>
-  </si>
-  <si>
-    <t>[0.019218333065509796]</t>
-  </si>
-  <si>
-    <t>[0.09568622708320618]</t>
-  </si>
-  <si>
-    <t>[0.2299012541770935]</t>
-  </si>
-  <si>
-    <t>[0.37834933400154114]</t>
-  </si>
-  <si>
-    <t>[-0.18188855051994324]</t>
-  </si>
-  <si>
-    <t>[0.22016851603984833]</t>
-  </si>
-  <si>
-    <t>[0.0486828088760376]</t>
-  </si>
-  <si>
-    <t>[-0.20169910788536072]</t>
-  </si>
-  <si>
-    <t>[0.3061114549636841]</t>
-  </si>
-  <si>
-    <t>[0.2628854513168335]</t>
-  </si>
-  <si>
-    <t>[-0.39054256677627563]</t>
-  </si>
-  <si>
-    <t>[-0.05377216637134552]</t>
-  </si>
-  <si>
-    <t>[0.021616440266370773]</t>
-  </si>
-  <si>
-    <t>[0.19422191381454468]</t>
-  </si>
-  <si>
-    <t>[0.0014161457074806094]</t>
-  </si>
-  <si>
-    <t>[-0.30043908953666687]</t>
-  </si>
-  <si>
-    <t>[-0.23348955810070038]</t>
-  </si>
-  <si>
-    <t>[-0.18967872858047485]</t>
-  </si>
-  <si>
-    <t>[-0.06621769070625305]</t>
-  </si>
-  <si>
-    <t>[-0.0064226677641272545]</t>
-  </si>
-  <si>
-    <t>[-0.07235316187143326]</t>
-  </si>
-  <si>
-    <t>[0.12866608798503876]</t>
-  </si>
-  <si>
-    <t>[0.039153311401605606]</t>
-  </si>
-  <si>
-    <t>[-0.12625432014465332]</t>
-  </si>
-  <si>
-    <t>[-0.1297461837530136]</t>
-  </si>
-  <si>
-    <t>[0.30553871393203735]</t>
-  </si>
-  <si>
-    <t>[0.14308877289295197]</t>
-  </si>
-  <si>
-    <t>[-0.00651406729593873]</t>
-  </si>
-  <si>
-    <t>[0.1302110105752945]</t>
-  </si>
-  <si>
-    <t>[-0.07780737429857254]</t>
-  </si>
-  <si>
-    <t>[0.2847210466861725]</t>
-  </si>
-  <si>
-    <t>[0.07731778919696808]</t>
-  </si>
-  <si>
-    <t>[-0.5732734799385071]</t>
-  </si>
-  <si>
-    <t>[-0.08659470081329346]</t>
-  </si>
-  <si>
-    <t>[-0.10362471640110016]</t>
-  </si>
-  <si>
-    <t>[0.41137275099754333]</t>
-  </si>
-  <si>
-    <t>[-0.048347461968660355]</t>
-  </si>
-  <si>
-    <t>[0.12054138630628586]</t>
-  </si>
-  <si>
-    <t>[0.05968073010444641]</t>
-  </si>
-  <si>
-    <t>[-0.08544907718896866]</t>
-  </si>
-  <si>
-    <t>[-0.010369133204221725]</t>
-  </si>
-  <si>
-    <t>[-0.06528717279434204]</t>
-  </si>
-  <si>
-    <t>[0.1939099282026291]</t>
-  </si>
-  <si>
-    <t>[-0.055371999740600586]</t>
-  </si>
-  <si>
-    <t>[-0.41418197751045227]</t>
-  </si>
-  <si>
-    <t>[0.09709593653678894]</t>
-  </si>
-  <si>
-    <t>[-0.1724882274866104]</t>
-  </si>
-  <si>
-    <t>[-0.20118381083011627]</t>
-  </si>
-  <si>
-    <t>[-0.19666500389575958]</t>
-  </si>
-  <si>
-    <t>[-0.25869035720825195]</t>
-  </si>
-  <si>
-    <t>[-0.3533336818218231]</t>
-  </si>
-  <si>
-    <t>[0.31380313634872437]</t>
-  </si>
-  <si>
-    <t>[-0.15016067028045654]</t>
-  </si>
-  <si>
-    <t>[0.09021983295679092]</t>
-  </si>
-  <si>
-    <t>[0.025118468329310417]</t>
-  </si>
-  <si>
-    <t>[0.1286221146583557]</t>
-  </si>
-  <si>
-    <t>[0.12628409266471863]</t>
-  </si>
-  <si>
-    <t>[0.2393926978111267]</t>
-  </si>
-  <si>
-    <t>[-0.18669432401657104]</t>
-  </si>
-  <si>
-    <t>[-0.5091950297355652]</t>
-  </si>
-  <si>
-    <t>[-0.09157507866621017]</t>
-  </si>
-  <si>
-    <t>[-0.0456763356924057]</t>
-  </si>
-  <si>
-    <t>[0.24390628933906555]</t>
-  </si>
-  <si>
-    <t>[-0.041977476328611374]</t>
-  </si>
-  <si>
-    <t>[-0.04989830031991005]</t>
-  </si>
-  <si>
-    <t>[0.06934494525194168]</t>
-  </si>
-  <si>
-    <t>[-0.26741087436676025]</t>
+    <t>[-0.3454302251338959]</t>
+  </si>
+  <si>
+    <t>[0.25008630752563477]</t>
+  </si>
+  <si>
+    <t>[-0.34760767221450806]</t>
+  </si>
+  <si>
+    <t>[0.06383044272661209]</t>
+  </si>
+  <si>
+    <t>[0.13815587759017944]</t>
+  </si>
+  <si>
+    <t>[0.18672195076942444]</t>
+  </si>
+  <si>
+    <t>[-0.2130109965801239]</t>
+  </si>
+  <si>
+    <t>[-0.12271144986152649]</t>
+  </si>
+  <si>
+    <t>[-0.09075945615768433]</t>
+  </si>
+  <si>
+    <t>[0.3252727687358856]</t>
+  </si>
+  <si>
+    <t>[-0.07043977081775665]</t>
+  </si>
+  <si>
+    <t>[-0.013292369432747364]</t>
+  </si>
+  <si>
+    <t>[0.33396580815315247]</t>
+  </si>
+  <si>
+    <t>[0.0193096324801445]</t>
+  </si>
+  <si>
+    <t>[0.05807627737522125]</t>
+  </si>
+  <si>
+    <t>[-0.2944813072681427]</t>
+  </si>
+  <si>
+    <t>[-0.1143551617860794]</t>
+  </si>
+  <si>
+    <t>[0.27482491731643677]</t>
+  </si>
+  <si>
+    <t>[0.15375638008117676]</t>
+  </si>
+  <si>
+    <t>[0.15436582267284393]</t>
+  </si>
+  <si>
+    <t>[-0.016055453568696976]</t>
+  </si>
+  <si>
+    <t>[-0.18052053451538086]</t>
+  </si>
+  <si>
+    <t>[-0.12693823873996735]</t>
+  </si>
+  <si>
+    <t>[-0.09565131366252899]</t>
+  </si>
+  <si>
+    <t>[-0.1933005452156067]</t>
+  </si>
+  <si>
+    <t>[0.3410857915878296]</t>
+  </si>
+  <si>
+    <t>[0.6332784295082092]</t>
+  </si>
+  <si>
+    <t>[-0.13937704265117645]</t>
+  </si>
+  <si>
+    <t>[0.05359500274062157]</t>
+  </si>
+  <si>
+    <t>[0.049570441246032715]</t>
+  </si>
+  <si>
+    <t>[0.006506273057311773]</t>
+  </si>
+  <si>
+    <t>[0.10012161731719971]</t>
+  </si>
+  <si>
+    <t>[-0.2344781458377838]</t>
+  </si>
+  <si>
+    <t>[0.026525776833295822]</t>
+  </si>
+  <si>
+    <t>[-0.190259650349617]</t>
+  </si>
+  <si>
+    <t>[0.16249293088912964]</t>
+  </si>
+  <si>
+    <t>[0.23259775340557098]</t>
+  </si>
+  <si>
+    <t>[-0.19966992735862732]</t>
+  </si>
+  <si>
+    <t>[0.03876294940710068]</t>
+  </si>
+  <si>
+    <t>[-0.4225866496562958]</t>
+  </si>
+  <si>
+    <t>[-0.3250620663166046]</t>
+  </si>
+  <si>
+    <t>[-0.12837189435958862]</t>
+  </si>
+  <si>
+    <t>[-0.03644511103630066]</t>
+  </si>
+  <si>
+    <t>[0.23641830682754517]</t>
+  </si>
+  <si>
+    <t>[0.0016762708546593785]</t>
+  </si>
+  <si>
+    <t>[0.05924345552921295]</t>
+  </si>
+  <si>
+    <t>[0.146633118391037]</t>
+  </si>
+  <si>
+    <t>[-0.2683008015155792]</t>
+  </si>
+  <si>
+    <t>[0.039025433361530304]</t>
+  </si>
+  <si>
+    <t>[0.01718500629067421]</t>
+  </si>
+  <si>
+    <t>[0.05466510355472565]</t>
+  </si>
+  <si>
+    <t>[0.4591139256954193]</t>
+  </si>
+  <si>
+    <t>[-0.19063003361225128]</t>
+  </si>
+  <si>
+    <t>[0.03774987533688545]</t>
+  </si>
+  <si>
+    <t>[0.02980811521410942]</t>
+  </si>
+  <si>
+    <t>[-0.09151818603277206]</t>
+  </si>
+  <si>
+    <t>[0.07955704629421234]</t>
+  </si>
+  <si>
+    <t>[0.1606273651123047]</t>
+  </si>
+  <si>
+    <t>[0.03216007724404335]</t>
+  </si>
+  <si>
+    <t>[-0.1827087551355362]</t>
+  </si>
+  <si>
+    <t>[-0.503960371017456]</t>
+  </si>
+  <si>
+    <t>[0.1219494417309761]</t>
+  </si>
+  <si>
+    <t>[-0.28223004937171936]</t>
+  </si>
+  <si>
+    <t>[0.18151378631591797]</t>
+  </si>
+  <si>
+    <t>[-0.11548250913619995]</t>
+  </si>
+  <si>
+    <t>[0.05142117664217949]</t>
+  </si>
+  <si>
+    <t>[-0.4878441393375397]</t>
+  </si>
+  <si>
+    <t>[0.2951480746269226]</t>
+  </si>
+  <si>
+    <t>[-0.18873727321624756]</t>
+  </si>
+  <si>
+    <t>[0.15522700548171997]</t>
+  </si>
+  <si>
+    <t>[0.0054845185950398445]</t>
+  </si>
+  <si>
+    <t>[0.18838919699192047]</t>
+  </si>
+  <si>
+    <t>[0.05883854255080223]</t>
+  </si>
+  <si>
+    <t>[-0.12391849607229233]</t>
+  </si>
+  <si>
+    <t>[-0.10859708487987518]</t>
+  </si>
+  <si>
+    <t>[0.10737096518278122]</t>
+  </si>
+  <si>
+    <t>[0.26175206899642944]</t>
+  </si>
+  <si>
+    <t>[0.19816192984580994]</t>
+  </si>
+  <si>
+    <t>[-0.23302914202213287]</t>
+  </si>
+  <si>
+    <t>[0.12271015346050262]</t>
+  </si>
+  <si>
+    <t>[-0.25523221492767334]</t>
+  </si>
+  <si>
+    <t>[0.3472060561180115]</t>
+  </si>
+  <si>
+    <t>[-0.36519157886505127]</t>
+  </si>
+  <si>
+    <t>[0.30089467763900757]</t>
+  </si>
+  <si>
+    <t>[-0.020570561289787292]</t>
+  </si>
+  <si>
+    <t>[0.07886553555727005]</t>
+  </si>
+  <si>
+    <t>[-0.1476721614599228]</t>
+  </si>
+  <si>
+    <t>[-0.20895802974700928]</t>
+  </si>
+  <si>
+    <t>[0.36800071597099304]</t>
+  </si>
+  <si>
+    <t>[-0.013018717058002949]</t>
+  </si>
+  <si>
+    <t>[0.2541114389896393]</t>
+  </si>
+  <si>
+    <t>[-0.25587695837020874]</t>
+  </si>
+  <si>
+    <t>[-0.23854829370975494]</t>
+  </si>
+  <si>
+    <t>[-0.08634965866804123]</t>
+  </si>
+  <si>
+    <t>[-0.009110362268984318]</t>
+  </si>
+  <si>
+    <t>[0.015705309808254242]</t>
+  </si>
+  <si>
+    <t>[0.19205157458782196]</t>
+  </si>
+  <si>
+    <t>[-0.5275338888168335]</t>
+  </si>
+  <si>
+    <t>[-0.3380071520805359]</t>
+  </si>
+  <si>
+    <t>[-0.10441625118255615]</t>
+  </si>
+  <si>
+    <t>[-0.08539789915084839]</t>
+  </si>
+  <si>
+    <t>[0.017168156802654266]</t>
+  </si>
+  <si>
+    <t>[0.19111555814743042]</t>
+  </si>
+  <si>
+    <t>[0.23029929399490356]</t>
+  </si>
+  <si>
+    <t>[-0.15238875150680542]</t>
+  </si>
+  <si>
+    <t>[0.1087021678686142]</t>
+  </si>
+  <si>
+    <t>[0.027263306081295013]</t>
+  </si>
+  <si>
+    <t>[-0.2603217661380768]</t>
+  </si>
+  <si>
+    <t>[-0.014455512166023254]</t>
+  </si>
+  <si>
+    <t>[0.1108558252453804]</t>
+  </si>
+  <si>
+    <t>[-0.16214844584465027]</t>
+  </si>
+  <si>
+    <t>[-0.09386032074689865]</t>
+  </si>
+  <si>
+    <t>[0.04380868375301361]</t>
+  </si>
+  <si>
+    <t>[-0.11569322645664215]</t>
+  </si>
+  <si>
+    <t>[-0.00985883828252554]</t>
+  </si>
+  <si>
+    <t>[-0.33400121331214905]</t>
+  </si>
+  <si>
+    <t>[-0.15596581995487213]</t>
+  </si>
+  <si>
+    <t>[-0.1429903358221054]</t>
+  </si>
+  <si>
+    <t>[0.2125655710697174]</t>
+  </si>
+  <si>
+    <t>[0.2831660211086273]</t>
+  </si>
+  <si>
+    <t>[-0.26241979002952576]</t>
+  </si>
+  <si>
+    <t>[-0.02013249695301056]</t>
+  </si>
+  <si>
+    <t>[-0.25061145424842834]</t>
+  </si>
+  <si>
+    <t>[0.16300299763679504]</t>
+  </si>
+  <si>
+    <t>[0.18813760578632355]</t>
+  </si>
+  <si>
+    <t>[0.2519732713699341]</t>
+  </si>
+  <si>
+    <t>[-0.03586755320429802]</t>
+  </si>
+  <si>
+    <t>[-0.2596384882926941]</t>
+  </si>
+  <si>
+    <t>[-0.2873200476169586]</t>
+  </si>
+  <si>
+    <t>[0.10153476893901825]</t>
+  </si>
+  <si>
+    <t>[-0.0860019326210022]</t>
+  </si>
+  <si>
+    <t>[0.1493522673845291]</t>
+  </si>
+  <si>
+    <t>[0.1484289914369583]</t>
+  </si>
+  <si>
+    <t>[0.04281572997570038]</t>
+  </si>
+  <si>
+    <t>[0.16557084023952484]</t>
+  </si>
+  <si>
+    <t>[0.25000953674316406]</t>
+  </si>
+  <si>
+    <t>[0.10423142462968826]</t>
+  </si>
+  <si>
+    <t>[-0.08069964498281479]</t>
+  </si>
+  <si>
+    <t>[0.43501046299934387]</t>
+  </si>
+  <si>
+    <t>[0.045013461261987686]</t>
+  </si>
+  <si>
+    <t>[0.15012283623218536]</t>
+  </si>
+  <si>
+    <t>[0.11465895920991898]</t>
+  </si>
+  <si>
+    <t>[-0.04331046715378761]</t>
+  </si>
+  <si>
+    <t>[-0.07017065584659576]</t>
+  </si>
+  <si>
+    <t>[0.47391295433044434]</t>
+  </si>
+  <si>
+    <t>[0.27148813009262085]</t>
+  </si>
+  <si>
+    <t>[0.0953204557299614]</t>
+  </si>
+  <si>
+    <t>[0.19461683928966522]</t>
+  </si>
+  <si>
+    <t>[0.04547505080699921]</t>
+  </si>
+  <si>
+    <t>[-0.24674174189567566]</t>
+  </si>
+  <si>
+    <t>[-0.1625521332025528]</t>
+  </si>
+  <si>
+    <t>[-0.07244651764631271]</t>
+  </si>
+  <si>
+    <t>[0.11499563604593277]</t>
+  </si>
+  <si>
+    <t>[0.01696106605231762]</t>
+  </si>
+  <si>
+    <t>[0.04947200044989586]</t>
+  </si>
+  <si>
+    <t>[-0.14526081085205078]</t>
+  </si>
+  <si>
+    <t>[-0.028501367196440697]</t>
+  </si>
+  <si>
+    <t>[-0.11098834127187729]</t>
+  </si>
+  <si>
+    <t>[-0.11027873307466507]</t>
+  </si>
+  <si>
+    <t>[0.23797650635242462]</t>
+  </si>
+  <si>
+    <t>[-0.40473249554634094]</t>
+  </si>
+  <si>
+    <t>[0.1998351663351059]</t>
+  </si>
+  <si>
+    <t>[-0.34089919924736023]</t>
+  </si>
+  <si>
+    <t>[0.41212043166160583]</t>
+  </si>
+  <si>
+    <t>[-0.11143699288368225]</t>
+  </si>
+  <si>
+    <t>[-0.08209393173456192]</t>
+  </si>
+  <si>
+    <t>[0.13731056451797485]</t>
+  </si>
+  <si>
+    <t>[-0.10270167142152786]</t>
+  </si>
+  <si>
+    <t>[-0.022785726934671402]</t>
+  </si>
+  <si>
+    <t>[0.018581336364150047]</t>
+  </si>
+  <si>
+    <t>[-0.10515061020851135]</t>
+  </si>
+  <si>
+    <t>[-0.0009442026494070888]</t>
+  </si>
+  <si>
+    <t>[0.3556109666824341]</t>
+  </si>
+  <si>
+    <t>[-0.31932204961776733]</t>
+  </si>
+  <si>
+    <t>[0.061746951192617416]</t>
+  </si>
+  <si>
+    <t>[0.25633764266967773]</t>
+  </si>
+  <si>
+    <t>[-0.03227498009800911]</t>
+  </si>
+  <si>
+    <t>[-0.20581458508968353]</t>
+  </si>
+  <si>
+    <t>[-0.15527424216270447]</t>
+  </si>
+  <si>
+    <t>[-0.03965242579579353]</t>
+  </si>
+  <si>
+    <t>[0.08635875582695007]</t>
+  </si>
+  <si>
+    <t>[-0.1618940234184265]</t>
+  </si>
+  <si>
+    <t>[-0.06070108339190483]</t>
+  </si>
+  <si>
+    <t>[-0.3026890456676483]</t>
+  </si>
+  <si>
+    <t>[-0.11739698052406311]</t>
+  </si>
+  <si>
+    <t>[0.29942891001701355]</t>
+  </si>
+  <si>
+    <t>[0.00022043292119633406]</t>
+  </si>
+  <si>
+    <t>[-0.5562899112701416]</t>
+  </si>
+  <si>
+    <t>[-0.15074211359024048]</t>
+  </si>
+  <si>
+    <t>[0.019193677231669426]</t>
+  </si>
+  <si>
+    <t>[0.09568742662668228]</t>
+  </si>
+  <si>
+    <t>[0.22989539802074432]</t>
+  </si>
+  <si>
+    <t>[0.3783510625362396]</t>
+  </si>
+  <si>
+    <t>[-0.18189316987991333]</t>
+  </si>
+  <si>
+    <t>[0.22017128765583038]</t>
+  </si>
+  <si>
+    <t>[0.048687782138586044]</t>
+  </si>
+  <si>
+    <t>[-0.20170025527477264]</t>
+  </si>
+  <si>
+    <t>[0.3061065077781677]</t>
+  </si>
+  <si>
+    <t>[0.26288625597953796]</t>
+  </si>
+  <si>
+    <t>[-0.3905400037765503]</t>
+  </si>
+  <si>
+    <t>[-0.05377582460641861]</t>
+  </si>
+  <si>
+    <t>[0.02160978503525257]</t>
+  </si>
+  <si>
+    <t>[0.19421613216400146]</t>
+  </si>
+  <si>
+    <t>[0.0014084642753005028]</t>
+  </si>
+  <si>
+    <t>[-0.3004538118839264]</t>
+  </si>
+  <si>
+    <t>[-0.23348557949066162]</t>
+  </si>
+  <si>
+    <t>[-0.18967056274414062]</t>
+  </si>
+  <si>
+    <t>[-0.06621693819761276]</t>
+  </si>
+  <si>
+    <t>[-0.006427830550819635]</t>
+  </si>
+  <si>
+    <t>[-0.0723569244146347]</t>
+  </si>
+  <si>
+    <t>[0.12866100668907166]</t>
+  </si>
+  <si>
+    <t>[0.03915039822459221]</t>
+  </si>
+  <si>
+    <t>[-0.12622962892055511]</t>
+  </si>
+  <si>
+    <t>[-0.1297479122877121]</t>
+  </si>
+  <si>
+    <t>[0.30552566051483154]</t>
+  </si>
+  <si>
+    <t>[0.14309203624725342]</t>
+  </si>
+  <si>
+    <t>[-0.006532042752951384]</t>
+  </si>
+  <si>
+    <t>[0.13020627200603485]</t>
+  </si>
+  <si>
+    <t>[-0.07781771570444107]</t>
+  </si>
+  <si>
+    <t>[0.284731388092041]</t>
+  </si>
+  <si>
+    <t>[0.0773046612739563]</t>
+  </si>
+  <si>
+    <t>[-0.5732643604278564]</t>
+  </si>
+  <si>
+    <t>[-0.08660471439361572]</t>
+  </si>
+  <si>
+    <t>[-0.10362005978822708]</t>
+  </si>
+  <si>
+    <t>[0.41137298941612244]</t>
+  </si>
+  <si>
+    <t>[-0.048351384699344635]</t>
+  </si>
+  <si>
+    <t>[0.12054196000099182]</t>
+  </si>
+  <si>
+    <t>[0.05967627093195915]</t>
+  </si>
+  <si>
+    <t>[-0.08544152230024338]</t>
+  </si>
+  <si>
+    <t>[-0.010357121005654335]</t>
+  </si>
+  <si>
+    <t>[-0.06529399007558823]</t>
+  </si>
+  <si>
+    <t>[0.19390706717967987]</t>
+  </si>
+  <si>
+    <t>[-0.05537886917591095]</t>
+  </si>
+  <si>
+    <t>[-0.4141841232776642]</t>
+  </si>
+  <si>
+    <t>[0.09708614647388458]</t>
+  </si>
+  <si>
+    <t>[-0.1724974364042282]</t>
+  </si>
+  <si>
+    <t>[-0.20120097696781158]</t>
+  </si>
+  <si>
+    <t>[-0.19666540622711182]</t>
+  </si>
+  <si>
+    <t>[-0.25868648290634155]</t>
+  </si>
+  <si>
+    <t>[-0.3533363938331604]</t>
+  </si>
+  <si>
+    <t>[0.3137904107570648]</t>
+  </si>
+  <si>
+    <t>[-0.15015430748462677]</t>
+  </si>
+  <si>
+    <t>[0.09020724147558212]</t>
+  </si>
+  <si>
+    <t>[0.025119194760918617]</t>
+  </si>
+  <si>
+    <t>[0.1286551058292389]</t>
+  </si>
+  <si>
+    <t>[0.12628836929798126]</t>
+  </si>
+  <si>
+    <t>[0.23937563598155975]</t>
+  </si>
+  <si>
+    <t>[-0.18669500946998596]</t>
+  </si>
+  <si>
+    <t>[-0.5092208385467529]</t>
+  </si>
+  <si>
+    <t>[-0.09158652275800705]</t>
+  </si>
+  <si>
+    <t>[-0.04569505527615547]</t>
+  </si>
+  <si>
+    <t>[0.24392147362232208]</t>
+  </si>
+  <si>
+    <t>[-0.04200304299592972]</t>
+  </si>
+  <si>
+    <t>[-0.0498708039522171]</t>
+  </si>
+  <si>
+    <t>[0.06934883445501328]</t>
+  </si>
+  <si>
+    <t>[-0.26740437746047974]</t>
   </si>
   <si>
     <t>b_i</t>
@@ -919,100 +919,100 @@
     <t>b_o</t>
   </si>
   <si>
-    <t>[-0.2784879803657532]</t>
-  </si>
-  <si>
-    <t>[1.237856149673462]</t>
-  </si>
-  <si>
-    <t>[-0.2667316496372223]</t>
-  </si>
-  <si>
-    <t>[0.21243524551391602]</t>
-  </si>
-  <si>
-    <t>[0.24530397355556488]</t>
-  </si>
-  <si>
-    <t>[1.121378779411316]</t>
-  </si>
-  <si>
-    <t>[-0.2281186282634735]</t>
-  </si>
-  <si>
-    <t>[-0.07686308771371841]</t>
-  </si>
-  <si>
-    <t>[-0.10812326520681381]</t>
-  </si>
-  <si>
-    <t>[1.0192359685897827]</t>
-  </si>
-  <si>
-    <t>[-0.11933264136314392]</t>
-  </si>
-  <si>
-    <t>[0.02515612728893757]</t>
-  </si>
-  <si>
-    <t>[0.22541013360023499]</t>
-  </si>
-  <si>
-    <t>[1.0455001592636108]</t>
-  </si>
-  <si>
-    <t>[-0.06231019273400307]</t>
-  </si>
-  <si>
-    <t>[0.08157237619161606]</t>
-  </si>
-  <si>
-    <t>[-0.11469408869743347]</t>
-  </si>
-  <si>
-    <t>[1.1013858318328857]</t>
-  </si>
-  <si>
-    <t>[-0.10090010613203049]</t>
-  </si>
-  <si>
-    <t>[0.04578177258372307]</t>
-  </si>
-  <si>
-    <t>[0.10453364253044128]</t>
-  </si>
-  <si>
-    <t>[1.0297212600708008]</t>
-  </si>
-  <si>
-    <t>[-0.1518048495054245]</t>
-  </si>
-  <si>
-    <t>[-0.02959175407886505]</t>
-  </si>
-  <si>
-    <t>[0.18156114220619202]</t>
-  </si>
-  <si>
-    <t>[1.1225403547286987]</t>
-  </si>
-  <si>
-    <t>[0.16439999639987946]</t>
-  </si>
-  <si>
-    <t>[-0.19021226465702057]</t>
-  </si>
-  <si>
-    <t>[-0.10150989145040512]</t>
-  </si>
-  <si>
-    <t>[1.0899401903152466]</t>
-  </si>
-  <si>
-    <t>[0.05915755778551102]</t>
-  </si>
-  <si>
-    <t>[0.09791721403598785]</t>
+    <t>[-0.278473436832428]</t>
+  </si>
+  <si>
+    <t>[1.2378493547439575]</t>
+  </si>
+  <si>
+    <t>[-0.26671916246414185]</t>
+  </si>
+  <si>
+    <t>[0.21243315935134888]</t>
+  </si>
+  <si>
+    <t>[0.24530890583992004]</t>
+  </si>
+  <si>
+    <t>[1.1214102506637573]</t>
+  </si>
+  <si>
+    <t>[-0.22812709212303162]</t>
+  </si>
+  <si>
+    <t>[-0.07685809582471848]</t>
+  </si>
+  <si>
+    <t>[-0.10812847316265106]</t>
+  </si>
+  <si>
+    <t>[1.0192338228225708]</t>
+  </si>
+  <si>
+    <t>[-0.11934589594602585]</t>
+  </si>
+  <si>
+    <t>[0.02514365129172802]</t>
+  </si>
+  <si>
+    <t>[0.22542133927345276]</t>
+  </si>
+  <si>
+    <t>[1.0455199480056763]</t>
+  </si>
+  <si>
+    <t>[-0.06230806186795235]</t>
+  </si>
+  <si>
+    <t>[0.08159381151199341]</t>
+  </si>
+  <si>
+    <t>[-0.11470584571361542]</t>
+  </si>
+  <si>
+    <t>[1.1013933420181274]</t>
+  </si>
+  <si>
+    <t>[-0.10091060400009155]</t>
+  </si>
+  <si>
+    <t>[0.045767493546009064]</t>
+  </si>
+  <si>
+    <t>[0.10452888160943985]</t>
+  </si>
+  <si>
+    <t>[1.0297220945358276]</t>
+  </si>
+  <si>
+    <t>[-0.151802659034729]</t>
+  </si>
+  <si>
+    <t>[-0.029584672302007675]</t>
+  </si>
+  <si>
+    <t>[0.18155568838119507]</t>
+  </si>
+  <si>
+    <t>[1.1225558519363403]</t>
+  </si>
+  <si>
+    <t>[0.1643991321325302]</t>
+  </si>
+  <si>
+    <t>[-0.19023257493972778]</t>
+  </si>
+  <si>
+    <t>[-0.10151395946741104]</t>
+  </si>
+  <si>
+    <t>[1.089945673942566]</t>
+  </si>
+  <si>
+    <t>[0.05918389931321144]</t>
+  </si>
+  <si>
+    <t>[0.097901351749897]</t>
   </si>
 </sst>
 </file>

</xml_diff>